<commit_message>
Refactor and web content update
</commit_message>
<xml_diff>
--- a/tabular/eve/hamaparvovirinae/epv-ichthama-refseqs-side-data.xlsx
+++ b/tabular/eve/hamaparvovirinae/epv-ichthama-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/hamaparvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB36EFFB-2FA6-8F43-96E5-221E270B728B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924F2D1B-D444-2943-AAA4-456AD36FED2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12360" yWindow="6440" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{2CCDC7F5-49D5-E94A-84D8-68DF3FAF2277}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
   <si>
     <t>sequenceID</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>ichthama.1-hippocampus</t>
+  </si>
+  <si>
+    <t>clade</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>Hippocampus comes</t>
+  </si>
+  <si>
+    <t>Serpentes (unranked)</t>
   </si>
 </sst>
 </file>
@@ -762,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CDEB45-2B2D-5640-8765-ED5799D7E31C}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:X3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="A1:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -772,6 +784,8 @@
     <col min="5" max="5" width="26.1640625" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" customWidth="1"/>
     <col min="9" max="9" width="22.1640625" customWidth="1"/>
+    <col min="19" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="20" width="17.83203125" customWidth="1"/>
     <col min="23" max="23" width="24.5" customWidth="1"/>
     <col min="24" max="24" width="28.83203125" customWidth="1"/>
   </cols>
@@ -906,8 +920,12 @@
         <v>22</v>
       </c>
       <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
+      <c r="T2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="V2" t="s">
         <v>28</v>
       </c>
@@ -974,8 +992,12 @@
         <v>22</v>
       </c>
       <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
+      <c r="T3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="V3" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added flanking data for ichthama-refseqs and proto-refseqs. Not done with protos
</commit_message>
<xml_diff>
--- a/tabular/eve/hamaparvovirinae/epv-ichthama-refseqs-side-data.xlsx
+++ b/tabular/eve/hamaparvovirinae/epv-ichthama-refseqs-side-data.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/hamaparvovirinae/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1F720B-F279-DD43-9619-8F5B3ABFC98C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="6440" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{2CCDC7F5-49D5-E94A-84D8-68DF3FAF2277}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
   <si>
     <t>sequenceID</t>
   </si>
@@ -160,12 +157,21 @@
   </si>
   <si>
     <t>ichthama.2-serpentes-UR</t>
+  </si>
+  <si>
+    <t>ENSHCOG00000009382</t>
+  </si>
+  <si>
+    <t>BHLHE23</t>
+  </si>
+  <si>
+    <t>YTHDF1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -317,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -369,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -563,26 +569,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8F3AFE-A2C5-2F46-9666-C9FF200A622E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C3" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -706,7 +712,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -767,18 +773,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CDEB45-2B2D-5640-8765-ED5799D7E31C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:X3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" customWidth="1"/>
@@ -790,7 +801,7 @@
     <col min="24" max="24" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,7 +875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
@@ -911,13 +922,13 @@
         <v>22</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>22</v>
+        <v>44</v>
+      </c>
+      <c r="R2" s="6">
+        <v>20</v>
       </c>
       <c r="S2" s="6"/>
       <c r="T2" s="6" t="s">
@@ -936,7 +947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
@@ -983,13 +994,13 @@
         <v>22</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="6" t="s">
-        <v>22</v>
+      <c r="R3" s="6">
+        <v>16</v>
       </c>
       <c r="S3" s="6"/>
       <c r="T3" s="6" t="s">
@@ -1010,5 +1021,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>